<commit_message>
đổi tên sheet không dấu
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/SME_Phu_luc.xlsx
+++ b/src/main/resources/templates/SME_Phu_luc.xlsx
@@ -4,10 +4,10 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="SL_ngay" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="KPIs ngay" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Tổng hợp" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="TLXLTB và PH" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Biểu đồ" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="KPI_ngay" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Tong_hop" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="TLXLTB_PH" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Bieu_Do" sheetId="5" r:id="rId8"/>
     <sheet state="hidden" name="TT Loi" sheetId="6" r:id="rId9"/>
     <sheet state="hidden" name="Tham chiếu" sheetId="7" r:id="rId10"/>
   </sheets>
@@ -2254,18 +2254,18 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Biểu đồ'!$C$13:$U$13</c:f>
+              <c:f>Bieu_Do!$C$13:$U$13</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Biểu đồ'!$C$14:$U$14</c:f>
+              <c:f>Bieu_Do!$C$14:$U$14</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1505132142"/>
-        <c:axId val="508988993"/>
+        <c:axId val="1366506824"/>
+        <c:axId val="1775361577"/>
       </c:barChart>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -2327,22 +2327,22 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Biểu đồ'!$C$13:$U$13</c:f>
+              <c:f>Bieu_Do!$C$13:$U$13</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Biểu đồ'!$C$15:$U$15</c:f>
+              <c:f>Bieu_Do!$C$15:$U$15</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1505132142"/>
-        <c:axId val="508988993"/>
+        <c:axId val="1366506824"/>
+        <c:axId val="1775361577"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1505132142"/>
+        <c:axId val="1366506824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2394,10 +2394,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508988993"/>
+        <c:crossAx val="1775361577"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="508988993"/>
+        <c:axId val="1775361577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2461,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505132142"/>
+        <c:crossAx val="1366506824"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -31756,15 +31756,15 @@
         <v>0.27</v>
       </c>
       <c r="D7" s="94">
-        <f>+'KPIs ngay'!$D$9</f>
+        <f>+KPI_ngay!$D$9</f>
         <v>1649584</v>
       </c>
       <c r="E7" s="94">
-        <f>+'KPIs ngay'!$D$8</f>
+        <f>+KPI_ngay!$D$8</f>
         <v>121</v>
       </c>
       <c r="F7" s="95">
-        <f>+'KPIs ngay'!$D$6</f>
+        <f>+KPI_ngay!$D$6</f>
         <v>0.02445060896</v>
       </c>
       <c r="G7" s="96">
@@ -31791,15 +31791,15 @@
         <v>2.0</v>
       </c>
       <c r="D8" s="94">
-        <f>+'KPIs ngay'!$D$14</f>
+        <f>+KPI_ngay!$D$14</f>
         <v>97764</v>
       </c>
       <c r="E8" s="94">
-        <f>+'KPIs ngay'!$D$13</f>
+        <f>+KPI_ngay!$D$13</f>
         <v>98</v>
       </c>
       <c r="F8" s="95">
-        <f>+'KPIs ngay'!$D$11</f>
+        <f>+KPI_ngay!$D$11</f>
         <v>0.3341379922</v>
       </c>
       <c r="G8" s="96">
@@ -31826,15 +31826,15 @@
         <v>2.8</v>
       </c>
       <c r="D9" s="94">
-        <f>+'KPIs ngay'!$D$19</f>
+        <f>+KPI_ngay!$D$19</f>
         <v>431497</v>
       </c>
       <c r="E9" s="94">
-        <f>+'KPIs ngay'!$D$18</f>
+        <f>+KPI_ngay!$D$18</f>
         <v>1808</v>
       </c>
       <c r="F9" s="95">
-        <f>+'KPIs ngay'!$D$16</f>
+        <f>+KPI_ngay!$D$16</f>
         <v>1.396687965</v>
       </c>
       <c r="G9" s="96">
@@ -31861,15 +31861,15 @@
         <v>2.7</v>
       </c>
       <c r="D10" s="94">
-        <f>+'KPIs ngay'!$D$24</f>
+        <f>+KPI_ngay!$D$24</f>
         <v>104369</v>
       </c>
       <c r="E10" s="94">
-        <f>+'KPIs ngay'!$D$23</f>
+        <f>+KPI_ngay!$D$23</f>
         <v>494</v>
       </c>
       <c r="F10" s="95">
-        <f>+'KPIs ngay'!$D$21</f>
+        <f>+KPI_ngay!$D$21</f>
         <v>1.577735407</v>
       </c>
       <c r="G10" s="96">
@@ -31972,11 +31972,11 @@
         <v>0.95</v>
       </c>
       <c r="D15" s="105">
-        <f>+'KPIs ngay'!$D$30</f>
+        <f>+KPI_ngay!$D$30</f>
         <v>123</v>
       </c>
       <c r="E15" s="105">
-        <f>+'KPIs ngay'!$D$29</f>
+        <f>+KPI_ngay!$D$29</f>
         <v>118</v>
       </c>
       <c r="F15" s="106">
@@ -32007,11 +32007,11 @@
         <v>0.95</v>
       </c>
       <c r="D16" s="105">
-        <f>+'KPIs ngay'!$D$35</f>
+        <f>+KPI_ngay!$D$35</f>
         <v>136</v>
       </c>
       <c r="E16" s="105">
-        <f>+'KPIs ngay'!$D$34</f>
+        <f>+KPI_ngay!$D$34</f>
         <v>130</v>
       </c>
       <c r="F16" s="106">
@@ -32042,11 +32042,11 @@
         <v>0.85</v>
       </c>
       <c r="D17" s="105">
-        <f>+'KPIs ngay'!$D$40</f>
+        <f>+KPI_ngay!$D$40</f>
         <v>1472</v>
       </c>
       <c r="E17" s="105">
-        <f>+'KPIs ngay'!$D$39</f>
+        <f>+KPI_ngay!$D$39</f>
         <v>588</v>
       </c>
       <c r="F17" s="106">
@@ -32077,11 +32077,11 @@
         <v>0.85</v>
       </c>
       <c r="D18" s="105">
-        <f>+'KPIs ngay'!$D$45</f>
+        <f>+KPI_ngay!$D$45</f>
         <v>461</v>
       </c>
       <c r="E18" s="105">
-        <f>+'KPIs ngay'!$D$44</f>
+        <f>+KPI_ngay!$D$44</f>
         <v>395</v>
       </c>
       <c r="F18" s="106">
@@ -32332,7 +32332,7 @@
         <v>1649584.0</v>
       </c>
       <c r="D27" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B27)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B27)</f>
         <v>0</v>
       </c>
       <c r="E27" s="130">
@@ -32344,7 +32344,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G27" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B27,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B27,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H27" s="131" t="str">
@@ -32356,7 +32356,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B27,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B27,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K27" s="130">
@@ -32382,7 +32382,7 @@
         <v>97764.0</v>
       </c>
       <c r="D28" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B28)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B28)</f>
         <v>0</v>
       </c>
       <c r="E28" s="130">
@@ -32394,7 +32394,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G28" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B28,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B28,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H28" s="131" t="str">
@@ -32406,7 +32406,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B28,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B28,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K28" s="130">
@@ -32432,7 +32432,7 @@
         <v>431497.0</v>
       </c>
       <c r="D29" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B29)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B29)</f>
         <v>0</v>
       </c>
       <c r="E29" s="130">
@@ -32444,7 +32444,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G29" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B29,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B29,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H29" s="131" t="str">
@@ -32456,7 +32456,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B29,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B29,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K29" s="130">
@@ -32482,7 +32482,7 @@
         <v>104369.0</v>
       </c>
       <c r="D30" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B30)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B30)</f>
         <v>0</v>
       </c>
       <c r="E30" s="130">
@@ -32494,7 +32494,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G30" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B30,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B30,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H30" s="131" t="str">
@@ -32506,7 +32506,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B30,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B30,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K30" s="130">
@@ -32532,7 +32532,7 @@
         <v>4272.0</v>
       </c>
       <c r="D31" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B31)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B31)</f>
         <v>0</v>
       </c>
       <c r="E31" s="130">
@@ -32544,7 +32544,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G31" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B31,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B31,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H31" s="131" t="str">
@@ -32556,7 +32556,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B31,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B31,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K31" s="130">
@@ -32582,7 +32582,7 @@
         <v>37000.0</v>
       </c>
       <c r="D32" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B32)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B32)</f>
         <v>0</v>
       </c>
       <c r="E32" s="130">
@@ -32594,7 +32594,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G32" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B32,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B32,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H32" s="131" t="str">
@@ -32606,7 +32606,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B32,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B32,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K32" s="130">
@@ -32632,7 +32632,7 @@
         <v>33156.0</v>
       </c>
       <c r="D33" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B33)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B33)</f>
         <v>0</v>
       </c>
       <c r="E33" s="130">
@@ -32644,7 +32644,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G33" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B33,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B33,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H33" s="131" t="str">
@@ -32656,7 +32656,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B33,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B33,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K33" s="130">
@@ -32682,7 +32682,7 @@
         <v>8505.0</v>
       </c>
       <c r="D34" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B34)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B34)</f>
         <v>0</v>
       </c>
       <c r="E34" s="130">
@@ -32694,7 +32694,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G34" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B34,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B34,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H34" s="131" t="str">
@@ -32706,7 +32706,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B34,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B34,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K34" s="130">
@@ -32730,7 +32730,7 @@
       </c>
       <c r="C35" s="129"/>
       <c r="D35" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B35)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B35)</f>
         <v>0</v>
       </c>
       <c r="E35" s="130">
@@ -32742,7 +32742,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G35" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B35,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B35,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H35" s="131" t="str">
@@ -32754,7 +32754,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B35,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B35,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K35" s="130">
@@ -32780,7 +32780,7 @@
         <v>1545.0</v>
       </c>
       <c r="D36" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B36)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B36)</f>
         <v>0</v>
       </c>
       <c r="E36" s="130">
@@ -32792,7 +32792,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G36" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B36,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B36,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H36" s="131" t="str">
@@ -32804,7 +32804,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B36,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B36,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K36" s="130">
@@ -32828,7 +32828,7 @@
       </c>
       <c r="C37" s="129"/>
       <c r="D37" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B37)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B37)</f>
         <v>0</v>
       </c>
       <c r="E37" s="130">
@@ -32840,7 +32840,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G37" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B37,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B37,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H37" s="131" t="str">
@@ -32852,7 +32852,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B37,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B37,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K37" s="130">
@@ -32878,7 +32878,7 @@
         <v>6572.0</v>
       </c>
       <c r="D38" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B38)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B38)</f>
         <v>0</v>
       </c>
       <c r="E38" s="130">
@@ -32890,7 +32890,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G38" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B38,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B38,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H38" s="131" t="str">
@@ -32902,7 +32902,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B38,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B38,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K38" s="130">
@@ -32926,7 +32926,7 @@
       </c>
       <c r="C39" s="129"/>
       <c r="D39" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B39)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B39)</f>
         <v>0</v>
       </c>
       <c r="E39" s="130">
@@ -32938,7 +32938,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G39" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B39,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B39,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H39" s="131" t="str">
@@ -32950,7 +32950,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B39,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B39,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K39" s="130">
@@ -32976,7 +32976,7 @@
         <v>572.0</v>
       </c>
       <c r="D40" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B40)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B40)</f>
         <v>0</v>
       </c>
       <c r="E40" s="130">
@@ -32988,7 +32988,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G40" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B40,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B40,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H40" s="131" t="str">
@@ -33000,7 +33000,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B40,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B40,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K40" s="130">
@@ -33026,7 +33026,7 @@
         <v>598.0</v>
       </c>
       <c r="D41" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B41)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B41)</f>
         <v>0</v>
       </c>
       <c r="E41" s="130">
@@ -33038,7 +33038,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G41" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B41,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B41,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H41" s="131" t="str">
@@ -33050,7 +33050,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B41,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B41,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K41" s="130">
@@ -33076,7 +33076,7 @@
         <v>1.0</v>
       </c>
       <c r="D42" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B42)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B42)</f>
         <v>0</v>
       </c>
       <c r="E42" s="130">
@@ -33088,7 +33088,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G42" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B42,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B42,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H42" s="131" t="str">
@@ -33100,7 +33100,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B42,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B42,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K42" s="130">
@@ -33126,7 +33126,7 @@
         <v>3841.0</v>
       </c>
       <c r="D43" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B43)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B43)</f>
         <v>0</v>
       </c>
       <c r="E43" s="130">
@@ -33138,7 +33138,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G43" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B43,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B43,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H43" s="131" t="str">
@@ -33150,7 +33150,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B43,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B43,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K43" s="130">
@@ -33176,7 +33176,7 @@
         <v>1369.0</v>
       </c>
       <c r="D44" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B44)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B44)</f>
         <v>0</v>
       </c>
       <c r="E44" s="130">
@@ -33188,7 +33188,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G44" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B44,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B44,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H44" s="131" t="str">
@@ -33200,7 +33200,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B44,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B44,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K44" s="130">
@@ -33226,7 +33226,7 @@
         <v>123.0</v>
       </c>
       <c r="D45" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B45)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B45)</f>
         <v>0</v>
       </c>
       <c r="E45" s="130">
@@ -33238,7 +33238,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G45" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B45,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B45,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H45" s="131" t="str">
@@ -33250,7 +33250,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B45,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B45,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K45" s="130">
@@ -33276,7 +33276,7 @@
         <v>5323.0</v>
       </c>
       <c r="D46" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B46)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B46)</f>
         <v>0</v>
       </c>
       <c r="E46" s="130">
@@ -33288,7 +33288,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G46" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B46,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B46,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H46" s="131" t="str">
@@ -33300,7 +33300,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B46,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B46,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K46" s="130">
@@ -33326,7 +33326,7 @@
         <v>274122.0</v>
       </c>
       <c r="D47" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B47)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B47)</f>
         <v>0</v>
       </c>
       <c r="E47" s="130">
@@ -33338,7 +33338,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G47" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B47,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B47,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H47" s="131" t="str">
@@ -33350,7 +33350,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B47,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B47,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K47" s="130">
@@ -33376,7 +33376,7 @@
         <v>55.0</v>
       </c>
       <c r="D48" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B48)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="130">
@@ -33388,7 +33388,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G48" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B48,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B48,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H48" s="131" t="str">
@@ -33400,7 +33400,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B48,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B48,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K48" s="130">
@@ -33424,7 +33424,7 @@
       </c>
       <c r="C49" s="129"/>
       <c r="D49" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B49)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B49)</f>
         <v>0</v>
       </c>
       <c r="E49" s="130">
@@ -33436,7 +33436,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G49" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B49,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B49,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H49" s="131" t="str">
@@ -33448,7 +33448,7 @@
         <v>0</v>
       </c>
       <c r="J49" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B49,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B49,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K49" s="130">
@@ -33469,7 +33469,7 @@
       </c>
       <c r="C50" s="129"/>
       <c r="D50" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B50)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B50)</f>
         <v>0</v>
       </c>
       <c r="E50" s="130">
@@ -33481,7 +33481,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G50" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B50,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B50,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H50" s="131" t="str">
@@ -33493,7 +33493,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B50,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B50,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K50" s="130">
@@ -33514,7 +33514,7 @@
       </c>
       <c r="C51" s="129"/>
       <c r="D51" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B51)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B51)</f>
         <v>0</v>
       </c>
       <c r="E51" s="130">
@@ -33526,7 +33526,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G51" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B51,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B51,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H51" s="131" t="str">
@@ -33538,7 +33538,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B51,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B51,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K51" s="130">
@@ -33559,7 +33559,7 @@
       </c>
       <c r="C52" s="129"/>
       <c r="D52" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B52)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B52)</f>
         <v>0</v>
       </c>
       <c r="E52" s="130">
@@ -33571,7 +33571,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G52" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B52,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B52,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H52" s="131" t="str">
@@ -33583,7 +33583,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B52,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B52,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K52" s="130">
@@ -33604,7 +33604,7 @@
       </c>
       <c r="C53" s="129"/>
       <c r="D53" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B53)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B53)</f>
         <v>0</v>
       </c>
       <c r="E53" s="130">
@@ -33616,7 +33616,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G53" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B53,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B53,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H53" s="131" t="str">
@@ -33628,7 +33628,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B53,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B53,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K53" s="130">
@@ -33649,7 +33649,7 @@
       </c>
       <c r="C54" s="129"/>
       <c r="D54" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B54)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B54)</f>
         <v>0</v>
       </c>
       <c r="E54" s="130">
@@ -33661,7 +33661,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G54" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B54,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B54,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H54" s="131" t="str">
@@ -33673,7 +33673,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B54,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B54,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K54" s="130">
@@ -33694,7 +33694,7 @@
       </c>
       <c r="C55" s="129"/>
       <c r="D55" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B55)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B55)</f>
         <v>0</v>
       </c>
       <c r="E55" s="130">
@@ -33706,7 +33706,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G55" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B55,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B55,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H55" s="131" t="str">
@@ -33718,7 +33718,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B55,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B55,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K55" s="130">
@@ -33739,7 +33739,7 @@
       </c>
       <c r="C56" s="129"/>
       <c r="D56" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B56)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B56)</f>
         <v>0</v>
       </c>
       <c r="E56" s="130">
@@ -33751,7 +33751,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G56" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B56,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B56,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H56" s="131" t="str">
@@ -33763,7 +33763,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B56,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B56,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K56" s="130">
@@ -33784,7 +33784,7 @@
       </c>
       <c r="C57" s="129"/>
       <c r="D57" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B57)</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B57)</f>
         <v>0</v>
       </c>
       <c r="E57" s="130">
@@ -33796,7 +33796,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G57" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B57,#REF!,"Báo lỗi")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B57,#REF!,"Báo lỗi")</f>
         <v>0</v>
       </c>
       <c r="H57" s="131" t="str">
@@ -33808,7 +33808,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="130">
-        <f>+COUNTIFS(#REF!,C$22,#REF!,'Tổng hợp'!$B57,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
+        <f>+COUNTIFS(#REF!,C$22,#REF!,Tong_hop!$B57,#REF!,"Báo lỗi",#REF!,"*Bất cập*")</f>
         <v>0</v>
       </c>
       <c r="K57" s="130">
@@ -35885,7 +35885,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B7)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B7)</f>
         <v>0</v>
       </c>
       <c r="D7" s="144">
@@ -35893,7 +35893,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B7),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B7),"-")</f>
         <v>-</v>
       </c>
       <c r="F7" s="144">
@@ -35909,11 +35909,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B7,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B7,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J7" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B7,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B7,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K7" s="146" t="str">
@@ -35925,7 +35925,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B7,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B7,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N7" s="5"/>
@@ -35950,7 +35950,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B8)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B8)</f>
         <v>0</v>
       </c>
       <c r="D8" s="144">
@@ -35958,7 +35958,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B8),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B8),"-")</f>
         <v>-</v>
       </c>
       <c r="F8" s="144">
@@ -35977,7 +35977,7 @@
         <v>65.0248</v>
       </c>
       <c r="J8" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B8,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B8,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K8" s="146" t="str">
@@ -35989,7 +35989,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B8,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B8,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N8" s="5"/>
@@ -36014,7 +36014,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B9)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B9)</f>
         <v>0</v>
       </c>
       <c r="D9" s="144">
@@ -36022,7 +36022,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B9),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B9),"-")</f>
         <v>-</v>
       </c>
       <c r="F9" s="144">
@@ -36038,11 +36038,11 @@
         <v>0</v>
       </c>
       <c r="I9" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B9,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B9,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J9" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B9,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B9,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K9" s="146" t="str">
@@ -36054,7 +36054,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B9,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B9,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N9" s="5"/>
@@ -36079,7 +36079,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B10)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B10)</f>
         <v>0</v>
       </c>
       <c r="D10" s="144">
@@ -36102,11 +36102,11 @@
         <v>0</v>
       </c>
       <c r="I10" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B10,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B10,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J10" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B10,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B10,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K10" s="146" t="str">
@@ -36118,7 +36118,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B10,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B10,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N10" s="5"/>
@@ -36143,7 +36143,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B11)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B11)</f>
         <v>0</v>
       </c>
       <c r="D11" s="144">
@@ -36151,7 +36151,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B11),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B11),"-")</f>
         <v>-</v>
       </c>
       <c r="F11" s="144">
@@ -36167,11 +36167,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B11,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B11,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J11" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B11,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B11,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K11" s="146" t="str">
@@ -36183,7 +36183,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B11,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B11,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N11" s="5"/>
@@ -36208,7 +36208,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B12)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B12)</f>
         <v>0</v>
       </c>
       <c r="D12" s="144">
@@ -36216,7 +36216,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B12),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B12),"-")</f>
         <v>-</v>
       </c>
       <c r="F12" s="144">
@@ -36232,11 +36232,11 @@
         <v>0</v>
       </c>
       <c r="I12" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B12,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B12,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J12" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B12,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B12,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K12" s="146" t="str">
@@ -36248,7 +36248,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B12,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B12,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N12" s="5"/>
@@ -36273,7 +36273,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B13)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B13)</f>
         <v>0</v>
       </c>
       <c r="D13" s="144">
@@ -36281,7 +36281,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B13),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B13),"-")</f>
         <v>-</v>
       </c>
       <c r="F13" s="144">
@@ -36297,11 +36297,11 @@
         <v>0</v>
       </c>
       <c r="I13" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B13,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B13,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J13" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B13,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B13,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K13" s="146" t="str">
@@ -36313,7 +36313,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B13,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B13,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N13" s="5"/>
@@ -36338,7 +36338,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B14)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B14)</f>
         <v>0</v>
       </c>
       <c r="D14" s="144">
@@ -36346,7 +36346,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B14),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B14),"-")</f>
         <v>-</v>
       </c>
       <c r="F14" s="144">
@@ -36362,11 +36362,11 @@
         <v>0</v>
       </c>
       <c r="I14" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B14,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B14,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J14" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B14,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B14,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K14" s="146" t="str">
@@ -36378,7 +36378,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B14,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B14,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N14" s="5"/>
@@ -36403,7 +36403,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B15)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B15)</f>
         <v>0</v>
       </c>
       <c r="D15" s="144">
@@ -36411,7 +36411,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B15),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B15),"-")</f>
         <v>-</v>
       </c>
       <c r="F15" s="144">
@@ -36427,11 +36427,11 @@
         <v>0</v>
       </c>
       <c r="I15" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B15,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B15,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J15" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B15,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B15,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K15" s="146" t="str">
@@ -36467,7 +36467,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B16)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B16)</f>
         <v>0</v>
       </c>
       <c r="D16" s="144">
@@ -36475,7 +36475,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B16),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B16),"-")</f>
         <v>-</v>
       </c>
       <c r="F16" s="144">
@@ -36491,11 +36491,11 @@
         <v>0</v>
       </c>
       <c r="I16" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B16,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B16,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J16" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B16,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B16,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K16" s="146" t="str">
@@ -36507,7 +36507,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B16,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B16,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N16" s="5"/>
@@ -36532,7 +36532,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B17)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B17)</f>
         <v>0</v>
       </c>
       <c r="D17" s="144">
@@ -36540,7 +36540,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B17),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B17),"-")</f>
         <v>-</v>
       </c>
       <c r="F17" s="144">
@@ -36556,11 +36556,11 @@
         <v>0</v>
       </c>
       <c r="I17" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B17,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B17,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J17" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B17,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B17,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K17" s="146" t="str">
@@ -36572,7 +36572,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B17,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B17,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N17" s="5"/>
@@ -36597,7 +36597,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B18)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B18)</f>
         <v>0</v>
       </c>
       <c r="D18" s="144">
@@ -36605,7 +36605,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B18),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B18),"-")</f>
         <v>-</v>
       </c>
       <c r="F18" s="144">
@@ -36621,11 +36621,11 @@
         <v>0</v>
       </c>
       <c r="I18" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B18,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B18,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J18" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B18,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B18,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K18" s="146" t="str">
@@ -36637,7 +36637,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B18,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B18,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N18" s="5"/>
@@ -36662,7 +36662,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B19)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B19)</f>
         <v>0</v>
       </c>
       <c r="D19" s="144">
@@ -36670,7 +36670,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B19),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B19),"-")</f>
         <v>-</v>
       </c>
       <c r="F19" s="144">
@@ -36689,7 +36689,7 @@
         <v>134</v>
       </c>
       <c r="J19" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B19,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B19,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K19" s="146" t="str">
@@ -36701,7 +36701,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B19,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B19,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N19" s="5"/>
@@ -36726,7 +36726,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B20)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B20)</f>
         <v>0</v>
       </c>
       <c r="D20" s="144">
@@ -36734,7 +36734,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B20),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B20),"-")</f>
         <v>-</v>
       </c>
       <c r="F20" s="144">
@@ -36750,11 +36750,11 @@
         <v>0</v>
       </c>
       <c r="I20" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B20,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B20,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J20" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B20,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B20,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K20" s="146" t="str">
@@ -36766,7 +36766,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B20,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B20,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N20" s="5"/>
@@ -36791,7 +36791,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B21)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B21)</f>
         <v>0</v>
       </c>
       <c r="D21" s="144">
@@ -36814,11 +36814,11 @@
         <v>0</v>
       </c>
       <c r="I21" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B21,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B21,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J21" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B21,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B21,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K21" s="146" t="str">
@@ -36830,7 +36830,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B21,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B21,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N21" s="5"/>
@@ -36855,7 +36855,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B22)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B22)</f>
         <v>0</v>
       </c>
       <c r="D22" s="144">
@@ -36863,7 +36863,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B22),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B22),"-")</f>
         <v>-</v>
       </c>
       <c r="F22" s="144">
@@ -36879,11 +36879,11 @@
         <v>0</v>
       </c>
       <c r="I22" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B22,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B22,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J22" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B22,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B22,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K22" s="146" t="str">
@@ -36919,7 +36919,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B23)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B23)</f>
         <v>0</v>
       </c>
       <c r="D23" s="144">
@@ -36927,7 +36927,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B23),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B23),"-")</f>
         <v>-</v>
       </c>
       <c r="F23" s="144">
@@ -36943,11 +36943,11 @@
         <v>0</v>
       </c>
       <c r="I23" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B23,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B23,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J23" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B23,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B23,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K23" s="146" t="str">
@@ -36959,7 +36959,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B23,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B23,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N23" s="5"/>
@@ -36984,7 +36984,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B24)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B24)</f>
         <v>0</v>
       </c>
       <c r="D24" s="144">
@@ -36992,7 +36992,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B24),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B24),"-")</f>
         <v>-</v>
       </c>
       <c r="F24" s="144">
@@ -37008,11 +37008,11 @@
         <v>0</v>
       </c>
       <c r="I24" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B24,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B24,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J24" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B24,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B24,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K24" s="146" t="str">
@@ -37024,7 +37024,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B24,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B24,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N24" s="5"/>
@@ -37049,7 +37049,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B25)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B25)</f>
         <v>0</v>
       </c>
       <c r="D25" s="144">
@@ -37057,7 +37057,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B25),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B25),"-")</f>
         <v>-</v>
       </c>
       <c r="F25" s="144">
@@ -37073,11 +37073,11 @@
         <v>0</v>
       </c>
       <c r="I25" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B25,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B25,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J25" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B25,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B25,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K25" s="146" t="str">
@@ -37089,7 +37089,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B25,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B25,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N25" s="5"/>
@@ -37114,7 +37114,7 @@
         <v>35</v>
       </c>
       <c r="C26" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B26)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B26)</f>
         <v>0</v>
       </c>
       <c r="D26" s="144">
@@ -37122,7 +37122,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B26),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B26),"-")</f>
         <v>-</v>
       </c>
       <c r="F26" s="144">
@@ -37138,11 +37138,11 @@
         <v>0</v>
       </c>
       <c r="I26" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B26,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B26,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J26" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B26,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B26,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K26" s="146" t="str">
@@ -37154,7 +37154,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B26,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B26,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N26" s="5"/>
@@ -37179,7 +37179,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B27)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B27)</f>
         <v>0</v>
       </c>
       <c r="D27" s="144">
@@ -37187,7 +37187,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B27),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B27),"-")</f>
         <v>-</v>
       </c>
       <c r="F27" s="144">
@@ -37203,11 +37203,11 @@
         <v>0</v>
       </c>
       <c r="I27" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B27,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B27,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J27" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B27,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B27,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K27" s="146" t="str">
@@ -37219,7 +37219,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B27,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B27,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N27" s="5"/>
@@ -37244,7 +37244,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B28)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B28)</f>
         <v>0</v>
       </c>
       <c r="D28" s="144">
@@ -37252,7 +37252,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B28),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B28),"-")</f>
         <v>-</v>
       </c>
       <c r="F28" s="144">
@@ -37268,11 +37268,11 @@
         <v>0</v>
       </c>
       <c r="I28" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B28,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B28,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J28" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B28,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B28,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K28" s="146" t="str">
@@ -37284,7 +37284,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B28,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B28,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N28" s="5"/>
@@ -37309,7 +37309,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B29)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B29)</f>
         <v>0</v>
       </c>
       <c r="D29" s="144">
@@ -37317,7 +37317,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B29),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B29),"-")</f>
         <v>-</v>
       </c>
       <c r="F29" s="144">
@@ -37333,11 +37333,11 @@
         <v>0</v>
       </c>
       <c r="I29" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B29,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B29,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J29" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B29,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B29,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K29" s="146" t="str">
@@ -37349,7 +37349,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B29,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B29,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N29" s="4"/>
@@ -37374,7 +37374,7 @@
         <v>39</v>
       </c>
       <c r="C30" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B30)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B30)</f>
         <v>0</v>
       </c>
       <c r="D30" s="144">
@@ -37382,7 +37382,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B30),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B30),"-")</f>
         <v>-</v>
       </c>
       <c r="F30" s="144">
@@ -37398,11 +37398,11 @@
         <v>0</v>
       </c>
       <c r="I30" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B30,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B30,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J30" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B30,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B30,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K30" s="146" t="str">
@@ -37414,7 +37414,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B30,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B30,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N30" s="4"/>
@@ -37439,7 +37439,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B31)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B31)</f>
         <v>0</v>
       </c>
       <c r="D31" s="144">
@@ -37447,7 +37447,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B31),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B31),"-")</f>
         <v>-</v>
       </c>
       <c r="F31" s="144">
@@ -37463,11 +37463,11 @@
         <v>0</v>
       </c>
       <c r="I31" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B31,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B31,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J31" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B31,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B31,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K31" s="146" t="str">
@@ -37479,7 +37479,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B31,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B31,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N31" s="4"/>
@@ -37504,7 +37504,7 @@
         <v>41</v>
       </c>
       <c r="C32" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B32)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B32)</f>
         <v>0</v>
       </c>
       <c r="D32" s="144">
@@ -37512,7 +37512,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B32),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B32),"-")</f>
         <v>-</v>
       </c>
       <c r="F32" s="144">
@@ -37528,11 +37528,11 @@
         <v>0</v>
       </c>
       <c r="I32" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B32,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B32,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J32" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B32,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B32,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K32" s="146" t="str">
@@ -37544,7 +37544,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B32,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B32,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N32" s="4"/>
@@ -37569,7 +37569,7 @@
         <v>42</v>
       </c>
       <c r="C33" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B33)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B33)</f>
         <v>0</v>
       </c>
       <c r="D33" s="144">
@@ -37577,7 +37577,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B33),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B33),"-")</f>
         <v>-</v>
       </c>
       <c r="F33" s="144">
@@ -37593,11 +37593,11 @@
         <v>0</v>
       </c>
       <c r="I33" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B33,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B33,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J33" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B33,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B33,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K33" s="146" t="str">
@@ -37609,7 +37609,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B33,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B33,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N33" s="4"/>
@@ -37634,7 +37634,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B34)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B34)</f>
         <v>0</v>
       </c>
       <c r="D34" s="144">
@@ -37642,7 +37642,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B34),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B34),"-")</f>
         <v>-</v>
       </c>
       <c r="F34" s="144">
@@ -37658,11 +37658,11 @@
         <v>0</v>
       </c>
       <c r="I34" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B34,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B34,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J34" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B34,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B34,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K34" s="146" t="str">
@@ -37674,7 +37674,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B34,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B34,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N34" s="4"/>
@@ -37699,7 +37699,7 @@
         <v>44</v>
       </c>
       <c r="C35" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B35)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B35)</f>
         <v>0</v>
       </c>
       <c r="D35" s="144">
@@ -37707,7 +37707,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B35),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B35),"-")</f>
         <v>-</v>
       </c>
       <c r="F35" s="144">
@@ -37723,11 +37723,11 @@
         <v>0</v>
       </c>
       <c r="I35" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B35,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B35,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J35" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B35,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B35,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K35" s="146" t="str">
@@ -37739,7 +37739,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B35,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B35,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N35" s="4"/>
@@ -37764,7 +37764,7 @@
         <v>45</v>
       </c>
       <c r="C36" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B36)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B36)</f>
         <v>0</v>
       </c>
       <c r="D36" s="144">
@@ -37772,7 +37772,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B36),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B36),"-")</f>
         <v>-</v>
       </c>
       <c r="F36" s="144">
@@ -37788,11 +37788,11 @@
         <v>0</v>
       </c>
       <c r="I36" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B36,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B36,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J36" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B36,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B36,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K36" s="146" t="str">
@@ -37804,7 +37804,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B36,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B36,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N36" s="4"/>
@@ -37829,7 +37829,7 @@
         <v>46</v>
       </c>
       <c r="C37" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B37)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B37)</f>
         <v>0</v>
       </c>
       <c r="D37" s="144">
@@ -37837,7 +37837,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B37),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B37),"-")</f>
         <v>-</v>
       </c>
       <c r="F37" s="144">
@@ -37853,11 +37853,11 @@
         <v>0</v>
       </c>
       <c r="I37" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B37,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B37,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J37" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B37,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B37,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K37" s="146" t="str">
@@ -37869,7 +37869,7 @@
         <v>0</v>
       </c>
       <c r="M37" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B37,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B37,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N37" s="4"/>
@@ -37894,7 +37894,7 @@
         <v>47</v>
       </c>
       <c r="C38" s="144">
-        <f>+COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B38)</f>
+        <f>+COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B38)</f>
         <v>0</v>
       </c>
       <c r="D38" s="144">
@@ -37902,7 +37902,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B38),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B38),"-")</f>
         <v>-</v>
       </c>
       <c r="F38" s="144">
@@ -37918,11 +37918,11 @@
         <v>0</v>
       </c>
       <c r="I38" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B38,#REF!,"&lt;&gt;0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B38,#REF!,"&lt;&gt;0"),"-")</f>
         <v>-</v>
       </c>
       <c r="J38" s="147">
-        <f>COUNTIFS(#REF!,C$3,#REF!,'TLXLTB và PH'!$B38,#REF!,"0")</f>
+        <f>COUNTIFS(#REF!,C$3,#REF!,TLXLTB_PH!$B38,#REF!,"0")</f>
         <v>0</v>
       </c>
       <c r="K38" s="146" t="str">
@@ -37934,7 +37934,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="145" t="str">
-        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,'TLXLTB và PH'!$B38,#REF!,"0"),"-")</f>
+        <f>IFERROR(AVERAGEIFS(#REF!,#REF!,C$3,#REF!,TLXLTB_PH!$B38,#REF!,"0"),"-")</f>
         <v>-</v>
       </c>
       <c r="N38" s="4"/>

</xml_diff>